<commit_message>
created forkJoin tasks, and tested it. results in spreadsheet
</commit_message>
<xml_diff>
--- a/StressTest.xlsx
+++ b/StressTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>rigidbody</t>
   </si>
@@ -37,6 +37,27 @@
   </si>
   <si>
     <t>CPU: intel i5-3450: 4 threads available</t>
+  </si>
+  <si>
+    <t>quad tree: maxObjs: 100, maxLevels: 5</t>
+  </si>
+  <si>
+    <t>ThreadList</t>
+  </si>
+  <si>
+    <t>forkJoin</t>
+  </si>
+  <si>
+    <t>1 threadList</t>
+  </si>
+  <si>
+    <t>2 threadList</t>
+  </si>
+  <si>
+    <t>4 threadList</t>
+  </si>
+  <si>
+    <t>8 threadList</t>
   </si>
 </sst>
 </file>
@@ -86,6 +107,1098 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.1148534847241008E-2"/>
+          <c:y val="9.5898026190374755E-2"/>
+          <c:w val="0.76434284921433282"/>
+          <c:h val="0.76498607276698904"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std loop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2266</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4693</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2290</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4731</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$10:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4731</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93118</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>535</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5280</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95948</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$10:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2323</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4662</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95635</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>forkJoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$10:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1446</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55906</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="105469440"/>
+        <c:axId val="106470720"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="105469440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="106470720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="106470720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="105469440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12704229906044356"/>
+          <c:y val="0.17823065206766558"/>
+          <c:w val="0.69332341189310087"/>
+          <c:h val="0.68722729068620358"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std loop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2266</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4693</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2290</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4731</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$10:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4731</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>535</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5280</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$10:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2323</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4662</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>forkJoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$10:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1446</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="79555584"/>
+        <c:axId val="82220672"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="79555584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82220672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="82220672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79555584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.81111054053025977"/>
+          <c:y val="0.25186374249649834"/>
+          <c:w val="0.1888894594697402"/>
+          <c:h val="0.49627215484612669"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="0"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.73228</cdr:x>
+      <cdr:y>0.91424</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.90088</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4059421" y="2538412"/>
+          <a:ext cx="934668" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>StressObjs</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00181</cdr:x>
+      <cdr:y>0.11321</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.06884</cdr:x>
+      <cdr:y>0.95197</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="9524" y="314325"/>
+          <a:ext cx="352425" cy="2328862"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" vert="vert" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>(microseconds)</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.35739</cdr:x>
+      <cdr:y>0.01372</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.65979</cdr:x>
+      <cdr:y>0.15094</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1981200" y="38100"/>
+          <a:ext cx="1676400" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Intel i5-3450</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,7 +1500,7 @@
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -395,123 +1508,149 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>8</v>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>100</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>394</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>615</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>445</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>535</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>402</v>
       </c>
+      <c r="G10">
+        <v>290</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>500</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>2266</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>2290</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>2297</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>2328</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>2323</v>
       </c>
+      <c r="G11">
+        <v>775</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>1000</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>4693</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>4731</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>4731</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>5280</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>4662</v>
       </c>
+      <c r="G12">
+        <v>1446</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>2500</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>99497</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>101799</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>93118</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>95948</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>95635</v>
+      </c>
+      <c r="G13">
+        <v>55906</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
stress test results from laptop
</commit_message>
<xml_diff>
--- a/StressTest.xlsx
+++ b/StressTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>rigidbody</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>8 threadList</t>
+  </si>
+  <si>
+    <t>CPU: intel i7-4710 8 threads available</t>
   </si>
 </sst>
 </file>
@@ -515,11 +518,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105469440"/>
-        <c:axId val="106470720"/>
+        <c:axId val="46423424"/>
+        <c:axId val="46433408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105469440"/>
+        <c:axId val="46423424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106470720"/>
+        <c:crossAx val="46433408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -537,7 +540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106470720"/>
+        <c:axId val="46433408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -548,7 +551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105469440"/>
+        <c:crossAx val="46423424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -656,15 +659,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="4"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$9</c:f>
+              <c:f>Sheet1!$E$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1 threadList</c:v>
+                  <c:v>4 threadList</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -692,18 +695,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$10:$C$12</c:f>
+              <c:f>Sheet1!$E$10:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>615</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2290</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4731</c:v>
+                  <c:v>535</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5280</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -711,15 +714,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="5"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$9</c:f>
+              <c:f>Sheet1!$F$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 threadList</c:v>
+                  <c:v>8 threadList</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -747,116 +750,6 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$10:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>445</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2297</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4731</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>4 threadList</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$10:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$10:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>535</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2328</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5280</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>8 threadList</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$10:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Sheet1!$F$10:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -877,7 +770,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="5"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$G$9</c:f>
@@ -940,11 +833,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="79555584"/>
-        <c:axId val="82220672"/>
+        <c:axId val="48702208"/>
+        <c:axId val="48703744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79555584"/>
+        <c:axId val="48702208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,7 +847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82220672"/>
+        <c:crossAx val="48703744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -962,7 +855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82220672"/>
+        <c:axId val="48703744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,7 +866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79555584"/>
+        <c:crossAx val="48702208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1006,6 +899,651 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std loop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1451</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>111666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3531</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117033</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$18:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>662</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3487</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>112633</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>forkJoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$18:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36033</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="38996608"/>
+        <c:axId val="38998400"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="38996608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="38998400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="38998400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="38996608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14459951881014874"/>
+          <c:y val="0.19028944298629338"/>
+          <c:w val="0.56808027121609794"/>
+          <c:h val="0.64280475357247013"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std loop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1451</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3518</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 threadList</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$18:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>662</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3487</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>forkJoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$18:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1225</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="65240064"/>
+        <c:axId val="65241856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="65240064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65241856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65241856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65240064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1049,16 +1587,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1074,6 +1612,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1193,6 +1791,317 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
             <a:t>Intel i5-3450</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00208</cdr:x>
+      <cdr:y>0.15046</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.08336</cdr:x>
+      <cdr:y>0.99942</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="9525" y="412750"/>
+          <a:ext cx="371584" cy="2328848"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vert="vert" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>(microseconds)</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.61111</cdr:x>
+      <cdr:y>0.90046</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.81554</cdr:x>
+      <cdr:y>0.98727</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2794000" y="2470150"/>
+          <a:ext cx="934642" cy="238116"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>StressObjs</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.27361</cdr:x>
+      <cdr:y>0.02199</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.64027</cdr:x>
+      <cdr:y>0.16088</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1250950" y="60325"/>
+          <a:ext cx="1676370" cy="380996"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Intel i7-4710</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -1488,10 +2397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,6 +2555,96 @@
       </c>
       <c r="G13">
         <v>55906</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>100</v>
+      </c>
+      <c r="B18">
+        <v>581</v>
+      </c>
+      <c r="C18">
+        <v>754</v>
+      </c>
+      <c r="D18">
+        <v>662</v>
+      </c>
+      <c r="E18">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>500</v>
+      </c>
+      <c r="B19">
+        <v>1451</v>
+      </c>
+      <c r="C19">
+        <v>1667</v>
+      </c>
+      <c r="D19">
+        <v>1662</v>
+      </c>
+      <c r="E19">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20">
+        <v>3518</v>
+      </c>
+      <c r="C20">
+        <v>3531</v>
+      </c>
+      <c r="D20">
+        <v>3487</v>
+      </c>
+      <c r="E20">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2500</v>
+      </c>
+      <c r="B21">
+        <v>111666</v>
+      </c>
+      <c r="C21">
+        <v>117033</v>
+      </c>
+      <c r="D21">
+        <v>112633</v>
+      </c>
+      <c r="E21">
+        <v>36033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>